<commit_message>
minor edits lesson 4, 6
</commit_message>
<xml_diff>
--- a/lessons/static/functions.xlsx
+++ b/lessons/static/functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/data-viz-notes/lessons/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D404E069-FBE7-454C-ACDC-7F64E41D1F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C24960E-5C7F-7747-B0CA-432132BB1233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{3A58871C-E590-B345-83F8-2E3F47B23569}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="152">
   <si>
     <t>Lesson</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t>Add a smoothing line to a scatter plot</t>
+  </si>
+  <si>
+    <t>gapminder</t>
+  </si>
+  <si>
+    <t>Life expectancy, population, and GDP by country</t>
   </si>
 </sst>
 </file>
@@ -836,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07006F67-71D7-DC4F-B2F9-77CFA3F8A29F}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1409,6 +1415,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>4</v>
+      </c>
       <c r="B30" t="s">
         <v>93</v>
       </c>
@@ -1770,6 +1779,23 @@
       </c>
       <c r="F49" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" t="s">
+        <v>151</v>
+      </c>
+      <c r="F50" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>